<commit_message>
ER diagram update and tables in excel
</commit_message>
<xml_diff>
--- a/Ideas.xlsx
+++ b/Ideas.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\file-alpha.campus.gla.ac.uk\scsc_group2\scsc_fs_student6\student\1002243W\ITECH project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dawwe\Desktop\Masters 2019-2020\Internet Tech\ITechGroupProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A43982-C860-4F9E-A1EE-EB1A7CCA2F85}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E666AE6F-CC27-4FA9-9357-63A65902266F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A4C79C33-EE3B-4DD3-8488-EB71656D6969}"/>
+    <workbookView xWindow="1644" yWindow="60" windowWidth="21300" windowHeight="10356" activeTab="1" xr2:uid="{A4C79C33-EE3B-4DD3-8488-EB71656D6969}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Rating" sheetId="2" r:id="rId2"/>
+    <sheet name="ER tables" sheetId="3" r:id="rId2"/>
+    <sheet name="Rating" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="89">
   <si>
     <t>Stuff to do</t>
   </si>
@@ -185,13 +186,127 @@
   </si>
   <si>
     <t>Focus should be on the creation and rating of playlist, not playing the music itself (link to Spotify, youtube etc, but don’t need to log in)</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>IntegerField(10)</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>CharField(30)</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>picture</t>
+  </si>
+  <si>
+    <t>FileField</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>songs</t>
+  </si>
+  <si>
+    <t>ForeignKey</t>
+  </si>
+  <si>
+    <t>artists</t>
+  </si>
+  <si>
+    <t>averageRating</t>
+  </si>
+  <si>
+    <t>FloatField</t>
+  </si>
+  <si>
+    <t>tags</t>
+  </si>
+  <si>
+    <t>oneToMany</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>playlist</t>
+  </si>
+  <si>
+    <t>attribute1</t>
+  </si>
+  <si>
+    <t>IntegerField(2)</t>
+  </si>
+  <si>
+    <t>attribute2</t>
+  </si>
+  <si>
+    <t>attribute3</t>
+  </si>
+  <si>
+    <t>Artist</t>
+  </si>
+  <si>
+    <t>webpage</t>
+  </si>
+  <si>
+    <t>URLField</t>
+  </si>
+  <si>
+    <t>linkToSpotify</t>
+  </si>
+  <si>
+    <t>numberOfPlaylists</t>
+  </si>
+  <si>
+    <t>IntegerField(5)</t>
+  </si>
+  <si>
+    <t>Song</t>
+  </si>
+  <si>
+    <t>artist</t>
+  </si>
+  <si>
+    <t>linkElsewhere</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>CharField(200)</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>DateField</t>
+  </si>
+  <si>
+    <t>ratings</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,6 +339,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -251,7 +382,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -428,11 +559,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -452,123 +598,129 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -883,24 +1035,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C27A730-BE19-432C-908B-66522BB6DBEC}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="98.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="98.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -908,7 +1061,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -916,7 +1069,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -924,153 +1077,153 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="49" t="s">
+      <c r="D11" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="51"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="27"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="52"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="54"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D12" s="28"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="30"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="52"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="54"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D14" s="52"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="54"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D15" s="52"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="53"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="54"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D16" s="52"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="53"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="54"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D13" s="28"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="30"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D14" s="28"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="30"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D15" s="28"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="30"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D16" s="28"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="30"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="52"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="54"/>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="28"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="30"/>
+    </row>
+    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="55"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="57"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D18" s="31"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="33"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -1085,21 +1238,553 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFFE657F-4CB3-438C-A631-8D51503531F5}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:S17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.77734375" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.77734375" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.77734375" customWidth="1"/>
+    <col min="11" max="11" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.77734375" customWidth="1"/>
+    <col min="14" max="14" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.77734375" customWidth="1"/>
+    <col min="17" max="17" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="58"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+    </row>
+    <row r="2" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="58"/>
+      <c r="B2" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="59"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="59"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="59"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="59" t="s">
+        <v>73</v>
+      </c>
+      <c r="L2" s="59"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="59" t="s">
+        <v>79</v>
+      </c>
+      <c r="O2" s="59"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="59" t="s">
+        <v>82</v>
+      </c>
+      <c r="R2" s="59"/>
+      <c r="S2" s="58"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="58"/>
+      <c r="B3" s="61" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="60" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="58"/>
+      <c r="E3" s="61" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="58"/>
+      <c r="H3" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="58"/>
+      <c r="K3" s="61" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="M3" s="58"/>
+      <c r="N3" s="61" t="s">
+        <v>59</v>
+      </c>
+      <c r="O3" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="61" t="s">
+        <v>83</v>
+      </c>
+      <c r="R3" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="S3" s="58"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="58"/>
+      <c r="B4" s="60" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="58"/>
+      <c r="E4" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="58"/>
+      <c r="H4" s="61" t="s">
+        <v>68</v>
+      </c>
+      <c r="I4" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" s="58"/>
+      <c r="K4" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="L4" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="M4" s="58"/>
+      <c r="N4" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="O4" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="P4" s="58"/>
+      <c r="Q4" s="60" t="s">
+        <v>77</v>
+      </c>
+      <c r="R4" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="S4" s="58"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="58"/>
+      <c r="B5" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="58"/>
+      <c r="E5" s="60" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="58"/>
+      <c r="H5" s="60" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="60" t="s">
+        <v>70</v>
+      </c>
+      <c r="J5" s="58"/>
+      <c r="K5" s="60" t="s">
+        <v>74</v>
+      </c>
+      <c r="L5" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="M5" s="58"/>
+      <c r="N5" s="60" t="s">
+        <v>76</v>
+      </c>
+      <c r="O5" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="P5" s="58"/>
+      <c r="Q5" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="R5" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="S5" s="58"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="58"/>
+      <c r="B6" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="60" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="58"/>
+      <c r="E6" s="60" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="60" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="58"/>
+      <c r="H6" s="60" t="s">
+        <v>71</v>
+      </c>
+      <c r="I6" s="60" t="s">
+        <v>70</v>
+      </c>
+      <c r="J6" s="58"/>
+      <c r="K6" s="60" t="s">
+        <v>76</v>
+      </c>
+      <c r="L6" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="M6" s="58"/>
+      <c r="N6" s="60" t="s">
+        <v>77</v>
+      </c>
+      <c r="O6" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="P6" s="58"/>
+      <c r="Q6" s="58"/>
+      <c r="R6" s="58"/>
+      <c r="S6" s="58"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="58"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="60" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="60" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" s="58"/>
+      <c r="H7" s="60" t="s">
+        <v>72</v>
+      </c>
+      <c r="I7" s="60" t="s">
+        <v>70</v>
+      </c>
+      <c r="J7" s="58"/>
+      <c r="K7" s="60" t="s">
+        <v>77</v>
+      </c>
+      <c r="L7" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="M7" s="58"/>
+      <c r="N7" s="60" t="s">
+        <v>81</v>
+      </c>
+      <c r="O7" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="P7" s="58"/>
+      <c r="Q7" s="58"/>
+      <c r="R7" s="58"/>
+      <c r="S7" s="58"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" s="58"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="58"/>
+      <c r="H8" s="60" t="s">
+        <v>84</v>
+      </c>
+      <c r="I8" s="60" t="s">
+        <v>85</v>
+      </c>
+      <c r="J8" s="58"/>
+      <c r="K8" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="L8" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="M8" s="58"/>
+      <c r="N8" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="O8" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="P8" s="58"/>
+      <c r="Q8" s="58"/>
+      <c r="R8" s="58"/>
+      <c r="S8" s="58"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" s="58"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="58"/>
+      <c r="H9" s="60" t="s">
+        <v>86</v>
+      </c>
+      <c r="I9" s="60" t="s">
+        <v>87</v>
+      </c>
+      <c r="J9" s="58"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="58"/>
+      <c r="M9" s="58"/>
+      <c r="N9" s="58"/>
+      <c r="O9" s="58"/>
+      <c r="P9" s="58"/>
+      <c r="Q9" s="58"/>
+      <c r="R9" s="58"/>
+      <c r="S9" s="58"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" s="58"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="58"/>
+      <c r="N10" s="58"/>
+      <c r="O10" s="58"/>
+      <c r="P10" s="58"/>
+      <c r="Q10" s="58"/>
+      <c r="R10" s="58"/>
+      <c r="S10" s="58"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="58"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="58"/>
+      <c r="M11" s="58"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="58"/>
+      <c r="P11" s="58"/>
+      <c r="Q11" s="58"/>
+      <c r="R11" s="58"/>
+      <c r="S11" s="58"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" s="58"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="58"/>
+      <c r="H12" s="58"/>
+      <c r="I12" s="58"/>
+      <c r="J12" s="58"/>
+      <c r="K12" s="58"/>
+      <c r="L12" s="58"/>
+      <c r="M12" s="58"/>
+      <c r="N12" s="58"/>
+      <c r="O12" s="58"/>
+      <c r="P12" s="58"/>
+      <c r="Q12" s="58"/>
+      <c r="R12" s="58"/>
+      <c r="S12" s="58"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" s="58"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58"/>
+      <c r="K13" s="58"/>
+      <c r="L13" s="58"/>
+      <c r="M13" s="58"/>
+      <c r="N13" s="58"/>
+      <c r="O13" s="58"/>
+      <c r="P13" s="58"/>
+      <c r="Q13" s="58"/>
+      <c r="R13" s="58"/>
+      <c r="S13" s="58"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14" s="58"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="58"/>
+      <c r="L14" s="58"/>
+      <c r="M14" s="58"/>
+      <c r="N14" s="58"/>
+      <c r="O14" s="58"/>
+      <c r="P14" s="58"/>
+      <c r="Q14" s="58"/>
+      <c r="R14" s="58"/>
+      <c r="S14" s="58"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" s="58"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="58"/>
+      <c r="G15" s="58"/>
+      <c r="H15" s="58"/>
+      <c r="I15" s="58"/>
+      <c r="J15" s="58"/>
+      <c r="K15" s="58"/>
+      <c r="L15" s="58"/>
+      <c r="M15" s="58"/>
+      <c r="N15" s="58"/>
+      <c r="O15" s="58"/>
+      <c r="P15" s="58"/>
+      <c r="S15" s="58"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" s="58"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="58"/>
+      <c r="K16" s="58"/>
+      <c r="L16" s="58"/>
+      <c r="M16" s="58"/>
+      <c r="N16" s="58"/>
+      <c r="O16" s="58"/>
+      <c r="P16" s="58"/>
+      <c r="S16" s="58"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" s="58"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="58"/>
+      <c r="L17" s="58"/>
+      <c r="M17" s="58"/>
+      <c r="N17" s="58"/>
+      <c r="O17" s="58"/>
+      <c r="P17" s="58"/>
+      <c r="S17" s="58"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E112665-A4DD-420C-8380-223FF5B10D2A}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:K29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="10" max="10" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B2" s="3"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -1111,7 +1796,7 @@
       <c r="J2" s="4"/>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -1123,7 +1808,7 @@
       <c r="J3" s="7"/>
       <c r="K3" s="8"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="6"/>
       <c r="C4" s="7" t="s">
         <v>26</v>
@@ -1137,7 +1822,7 @@
       <c r="J4" s="7"/>
       <c r="K4" s="8"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" s="6"/>
       <c r="C5" s="7" t="s">
         <v>27</v>
@@ -1151,7 +1836,7 @@
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
         <v>28</v>
@@ -1165,7 +1850,7 @@
       <c r="J6" s="7"/>
       <c r="K6" s="8"/>
     </row>
-    <row r="7" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="6"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -1177,7 +1862,7 @@
       <c r="J7" s="7"/>
       <c r="K7" s="8"/>
     </row>
-    <row r="8" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="6"/>
       <c r="C8" s="12" t="s">
         <v>42</v>
@@ -1191,7 +1876,7 @@
       <c r="J8" s="14"/>
       <c r="K8" s="8"/>
     </row>
-    <row r="9" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="6"/>
       <c r="C9" s="15" t="s">
         <v>43</v>
@@ -1209,61 +1894,61 @@
       </c>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="6"/>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="35" t="s">
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="J10" s="32" t="s">
+      <c r="J10" s="43" t="s">
         <v>44</v>
       </c>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="6"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="33"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="44"/>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="6"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="33"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="44"/>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="6"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="34"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="45"/>
       <c r="K13" s="8"/>
     </row>
-    <row r="14" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="6"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -1275,7 +1960,7 @@
       <c r="J14" s="7"/>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
       <c r="C15" s="15" t="s">
         <v>29</v>
@@ -1293,187 +1978,187 @@
       </c>
       <c r="K15" s="8"/>
     </row>
-    <row r="16" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="38" t="s">
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="J16" s="39" t="s">
+      <c r="J16" s="24" t="s">
         <v>37</v>
       </c>
       <c r="K16" s="8"/>
     </row>
-    <row r="17" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="6"/>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="38" t="s">
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="J17" s="39" t="s">
+      <c r="J17" s="24" t="s">
         <v>38</v>
       </c>
       <c r="K17" s="8"/>
     </row>
-    <row r="18" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="6"/>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="38" t="s">
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="J18" s="39" t="s">
+      <c r="J18" s="24" t="s">
         <v>49</v>
       </c>
       <c r="K18" s="8"/>
     </row>
-    <row r="19" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="6"/>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="38" t="s">
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="53"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J19" s="39" t="s">
+      <c r="J19" s="24" t="s">
         <v>48</v>
       </c>
       <c r="K19" s="8"/>
     </row>
-    <row r="20" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="6"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="27"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="20"/>
       <c r="K20" s="8"/>
     </row>
-    <row r="21" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="6"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="27"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="50"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="20"/>
       <c r="K21" s="8"/>
     </row>
-    <row r="22" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="6"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="27"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="50"/>
+      <c r="H22" s="51"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="20"/>
       <c r="K22" s="8"/>
     </row>
-    <row r="23" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="6"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="27"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="50"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="20"/>
       <c r="K23" s="8"/>
     </row>
-    <row r="24" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="6"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="27"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="50"/>
+      <c r="H24" s="51"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="20"/>
       <c r="K24" s="8"/>
     </row>
-    <row r="25" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="6"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="27"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="51"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="20"/>
       <c r="K25" s="8"/>
     </row>
-    <row r="26" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="6"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="27"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="51"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="20"/>
       <c r="K26" s="8"/>
     </row>
-    <row r="27" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="6"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="27"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="20"/>
       <c r="K27" s="8"/>
     </row>
-    <row r="28" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="6"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="29"/>
+      <c r="C28" s="52"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="22"/>
       <c r="K28" s="8"/>
     </row>
-    <row r="29" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="9"/>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
@@ -1487,16 +2172,16 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="C25:H25"/>
     <mergeCell ref="C10:H13"/>
     <mergeCell ref="J10:J13"/>
     <mergeCell ref="I10:I13"/>
     <mergeCell ref="C26:H26"/>
     <mergeCell ref="C27:H27"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="C24:H24"/>
-    <mergeCell ref="C25:H25"/>
     <mergeCell ref="C16:H16"/>
     <mergeCell ref="C17:H17"/>
     <mergeCell ref="C18:H18"/>

</xml_diff>

<commit_message>
Chen tables updated with extra categories
</commit_message>
<xml_diff>
--- a/Ideas.xlsx
+++ b/Ideas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dawwe\Desktop\Masters 2019-2020\Internet Tech\ITechGroupProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E666AE6F-CC27-4FA9-9357-63A65902266F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D068D0-7F50-490D-90CC-AEC0DA7C9775}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1644" yWindow="60" windowWidth="21300" windowHeight="10356" activeTab="1" xr2:uid="{A4C79C33-EE3B-4DD3-8488-EB71656D6969}"/>
+    <workbookView xWindow="504" yWindow="432" windowWidth="21300" windowHeight="10356" activeTab="1" xr2:uid="{A4C79C33-EE3B-4DD3-8488-EB71656D6969}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="93">
   <si>
     <t>Stuff to do</t>
   </si>
@@ -194,9 +194,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>IntegerField(10)</t>
-  </si>
-  <si>
     <t>username</t>
   </si>
   <si>
@@ -300,6 +297,21 @@
   </si>
   <si>
     <t>ratings</t>
+  </si>
+  <si>
+    <t>IntegerField(6)</t>
+  </si>
+  <si>
+    <t>IntegerField(8)</t>
+  </si>
+  <si>
+    <t>createdDate</t>
+  </si>
+  <si>
+    <t>lastUpdated</t>
+  </si>
+  <si>
+    <t>numberOfRatings</t>
   </si>
 </sst>
 </file>
@@ -578,7 +590,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -616,111 +628,112 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1101,82 +1114,82 @@
       <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="27"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="31"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="30"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="34"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="30"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="34"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D14" s="28"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="30"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="34"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D15" s="28"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="30"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="34"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D16" s="28"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="30"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="34"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="28"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="30"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="34"/>
     </row>
     <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="31"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="33"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="37"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
@@ -1240,10 +1253,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFFE657F-4CB3-438C-A631-8D51503531F5}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1251,8 +1264,8 @@
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
     <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.77734375" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3.77734375" customWidth="1"/>
     <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
@@ -1268,499 +1281,509 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="58"/>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="58"/>
+      <c r="A1" s="25"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
     </row>
     <row r="2" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="58"/>
-      <c r="B2" s="59" t="s">
+      <c r="A2" s="25"/>
+      <c r="B2" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="59" t="s">
+      <c r="C2" s="26"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="59"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="59" t="s">
+      <c r="F2" s="26"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="59"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="59" t="s">
+      <c r="I2" s="26"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="L2" s="26"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="O2" s="26"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="R2" s="26"/>
+      <c r="S2" s="25"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="25"/>
+      <c r="B3" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="25"/>
+      <c r="E3" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G3" s="25"/>
+      <c r="H3" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="25"/>
+      <c r="K3" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="M3" s="25"/>
+      <c r="N3" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="O3" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="R3" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="S3" s="25"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="25"/>
+      <c r="B4" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="25"/>
+      <c r="E4" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="25"/>
+      <c r="H4" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="25"/>
+      <c r="K4" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="L4" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="M4" s="25"/>
+      <c r="N4" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="O4" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="R4" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="S4" s="25"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="25"/>
+      <c r="B5" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="25"/>
+      <c r="E5" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="25"/>
+      <c r="H5" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="J5" s="25"/>
+      <c r="K5" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="L2" s="59"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="59" t="s">
-        <v>79</v>
-      </c>
-      <c r="O2" s="59"/>
-      <c r="P2" s="58"/>
-      <c r="Q2" s="59" t="s">
-        <v>82</v>
-      </c>
-      <c r="R2" s="59"/>
-      <c r="S2" s="58"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="58"/>
-      <c r="B3" s="61" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="60" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="58"/>
-      <c r="E3" s="61" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="G3" s="58"/>
-      <c r="H3" s="61" t="s">
-        <v>67</v>
-      </c>
-      <c r="I3" s="60" t="s">
+      <c r="L5" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="M5" s="25"/>
+      <c r="N5" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="O5" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="25"/>
+      <c r="S5" s="25"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="25"/>
+      <c r="B6" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="25"/>
+      <c r="E6" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="J3" s="58"/>
-      <c r="K3" s="61" t="s">
-        <v>59</v>
-      </c>
-      <c r="L3" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="M3" s="58"/>
-      <c r="N3" s="61" t="s">
-        <v>59</v>
-      </c>
-      <c r="O3" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="P3" s="58"/>
-      <c r="Q3" s="61" t="s">
+      <c r="F6" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="25"/>
+      <c r="H6" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="J6" s="25"/>
+      <c r="K6" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="L6" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="M6" s="25"/>
+      <c r="N6" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="O6" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="25"/>
+      <c r="S6" s="25"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="25"/>
+      <c r="H7" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7" s="25"/>
+      <c r="K7" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="L7" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="M7" s="25"/>
+      <c r="N7" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="O7" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="25"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="25"/>
+      <c r="H8" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="R3" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="S3" s="58"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="58"/>
-      <c r="B4" s="60" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" s="58"/>
-      <c r="E4" s="60" t="s">
+      <c r="I8" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25"/>
+      <c r="S8" s="25"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="G4" s="58"/>
-      <c r="H4" s="61" t="s">
-        <v>68</v>
-      </c>
-      <c r="I4" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="J4" s="58"/>
-      <c r="K4" s="60" t="s">
+      <c r="G9" s="25"/>
+      <c r="H9" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="25"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="L4" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="M4" s="58"/>
-      <c r="N4" s="61" t="s">
-        <v>80</v>
-      </c>
-      <c r="O4" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="P4" s="58"/>
-      <c r="Q4" s="60" t="s">
-        <v>77</v>
-      </c>
-      <c r="R4" s="60" t="s">
-        <v>78</v>
-      </c>
-      <c r="S4" s="58"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="58"/>
-      <c r="B5" s="60" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" s="58"/>
-      <c r="E5" s="60" t="s">
-        <v>62</v>
-      </c>
-      <c r="F5" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="G5" s="58"/>
-      <c r="H5" s="60" t="s">
-        <v>69</v>
-      </c>
-      <c r="I5" s="60" t="s">
-        <v>70</v>
-      </c>
-      <c r="J5" s="58"/>
-      <c r="K5" s="60" t="s">
-        <v>74</v>
-      </c>
-      <c r="L5" s="60" t="s">
-        <v>75</v>
-      </c>
-      <c r="M5" s="58"/>
-      <c r="N5" s="60" t="s">
-        <v>76</v>
-      </c>
-      <c r="O5" s="60" t="s">
-        <v>75</v>
-      </c>
-      <c r="P5" s="58"/>
-      <c r="Q5" s="60" t="s">
-        <v>68</v>
-      </c>
-      <c r="R5" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="S5" s="58"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="58"/>
-      <c r="B6" s="60" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="60" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="58"/>
-      <c r="E6" s="60" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" s="60" t="s">
-        <v>64</v>
-      </c>
-      <c r="G6" s="58"/>
-      <c r="H6" s="60" t="s">
-        <v>71</v>
-      </c>
-      <c r="I6" s="60" t="s">
-        <v>70</v>
-      </c>
-      <c r="J6" s="58"/>
-      <c r="K6" s="60" t="s">
-        <v>76</v>
-      </c>
-      <c r="L6" s="60" t="s">
-        <v>75</v>
-      </c>
-      <c r="M6" s="58"/>
-      <c r="N6" s="60" t="s">
-        <v>77</v>
-      </c>
-      <c r="O6" s="60" t="s">
-        <v>78</v>
-      </c>
-      <c r="P6" s="58"/>
-      <c r="Q6" s="58"/>
-      <c r="R6" s="58"/>
-      <c r="S6" s="58"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="58"/>
-      <c r="B7" s="58"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="60" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7" s="60" t="s">
-        <v>66</v>
-      </c>
-      <c r="G7" s="58"/>
-      <c r="H7" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="I7" s="60" t="s">
-        <v>70</v>
-      </c>
-      <c r="J7" s="58"/>
-      <c r="K7" s="60" t="s">
-        <v>77</v>
-      </c>
-      <c r="L7" s="60" t="s">
-        <v>78</v>
-      </c>
-      <c r="M7" s="58"/>
-      <c r="N7" s="60" t="s">
-        <v>81</v>
-      </c>
-      <c r="O7" s="60" t="s">
-        <v>75</v>
-      </c>
-      <c r="P7" s="58"/>
-      <c r="Q7" s="58"/>
-      <c r="R7" s="58"/>
-      <c r="S7" s="58"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="58"/>
-      <c r="B8" s="58"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="60" t="s">
-        <v>88</v>
-      </c>
-      <c r="F8" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="G8" s="58"/>
-      <c r="H8" s="60" t="s">
-        <v>84</v>
-      </c>
-      <c r="I8" s="60" t="s">
-        <v>85</v>
-      </c>
-      <c r="J8" s="58"/>
-      <c r="K8" s="60" t="s">
-        <v>68</v>
-      </c>
-      <c r="L8" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="M8" s="58"/>
-      <c r="N8" s="60" t="s">
-        <v>68</v>
-      </c>
-      <c r="O8" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="P8" s="58"/>
-      <c r="Q8" s="58"/>
-      <c r="R8" s="58"/>
-      <c r="S8" s="58"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="58"/>
-      <c r="B9" s="58"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="60" t="s">
-        <v>67</v>
-      </c>
-      <c r="F9" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="G9" s="58"/>
-      <c r="H9" s="60" t="s">
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="25"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="I9" s="60" t="s">
-        <v>87</v>
-      </c>
-      <c r="J9" s="58"/>
-      <c r="K9" s="58"/>
-      <c r="L9" s="58"/>
-      <c r="M9" s="58"/>
-      <c r="N9" s="58"/>
-      <c r="O9" s="58"/>
-      <c r="P9" s="58"/>
-      <c r="Q9" s="58"/>
-      <c r="R9" s="58"/>
-      <c r="S9" s="58"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="58"/>
-      <c r="B10" s="58"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
-      <c r="H10" s="58"/>
-      <c r="I10" s="58"/>
-      <c r="J10" s="58"/>
-      <c r="K10" s="58"/>
-      <c r="L10" s="58"/>
-      <c r="M10" s="58"/>
-      <c r="N10" s="58"/>
-      <c r="O10" s="58"/>
-      <c r="P10" s="58"/>
-      <c r="Q10" s="58"/>
-      <c r="R10" s="58"/>
-      <c r="S10" s="58"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="58"/>
-      <c r="B11" s="58"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="58"/>
-      <c r="G11" s="58"/>
-      <c r="H11" s="58"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="58"/>
-      <c r="K11" s="58"/>
-      <c r="L11" s="58"/>
-      <c r="M11" s="58"/>
-      <c r="N11" s="58"/>
-      <c r="O11" s="58"/>
-      <c r="P11" s="58"/>
-      <c r="Q11" s="58"/>
-      <c r="R11" s="58"/>
-      <c r="S11" s="58"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="25"/>
+      <c r="S11" s="25"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" s="58"/>
-      <c r="B12" s="58"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="58"/>
-      <c r="H12" s="58"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="58"/>
-      <c r="K12" s="58"/>
-      <c r="L12" s="58"/>
-      <c r="M12" s="58"/>
-      <c r="N12" s="58"/>
-      <c r="O12" s="58"/>
-      <c r="P12" s="58"/>
-      <c r="Q12" s="58"/>
-      <c r="R12" s="58"/>
-      <c r="S12" s="58"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="25"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="58"/>
-      <c r="B13" s="58"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="58"/>
-      <c r="F13" s="58"/>
-      <c r="G13" s="58"/>
-      <c r="H13" s="58"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="58"/>
-      <c r="K13" s="58"/>
-      <c r="L13" s="58"/>
-      <c r="M13" s="58"/>
-      <c r="N13" s="58"/>
-      <c r="O13" s="58"/>
-      <c r="P13" s="58"/>
-      <c r="Q13" s="58"/>
-      <c r="R13" s="58"/>
-      <c r="S13" s="58"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="25"/>
+      <c r="R13" s="25"/>
+      <c r="S13" s="25"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="58"/>
-      <c r="B14" s="58"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="58"/>
-      <c r="G14" s="58"/>
-      <c r="H14" s="58"/>
-      <c r="I14" s="58"/>
-      <c r="J14" s="58"/>
-      <c r="K14" s="58"/>
-      <c r="L14" s="58"/>
-      <c r="M14" s="58"/>
-      <c r="N14" s="58"/>
-      <c r="O14" s="58"/>
-      <c r="P14" s="58"/>
-      <c r="Q14" s="58"/>
-      <c r="R14" s="58"/>
-      <c r="S14" s="58"/>
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="25"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="25"/>
+      <c r="R14" s="25"/>
+      <c r="S14" s="25"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="58"/>
-      <c r="B15" s="58"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="58"/>
-      <c r="G15" s="58"/>
-      <c r="H15" s="58"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="58"/>
-      <c r="K15" s="58"/>
-      <c r="L15" s="58"/>
-      <c r="M15" s="58"/>
-      <c r="N15" s="58"/>
-      <c r="O15" s="58"/>
-      <c r="P15" s="58"/>
-      <c r="S15" s="58"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="25"/>
+      <c r="N15" s="25"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="25"/>
+      <c r="S15" s="25"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="58"/>
-      <c r="B16" s="58"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="58"/>
-      <c r="G16" s="58"/>
-      <c r="H16" s="58"/>
-      <c r="I16" s="58"/>
-      <c r="J16" s="58"/>
-      <c r="K16" s="58"/>
-      <c r="L16" s="58"/>
-      <c r="M16" s="58"/>
-      <c r="N16" s="58"/>
-      <c r="O16" s="58"/>
-      <c r="P16" s="58"/>
-      <c r="S16" s="58"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="25"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="25"/>
+      <c r="S16" s="25"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A17" s="58"/>
-      <c r="B17" s="58"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="58"/>
-      <c r="I17" s="58"/>
-      <c r="J17" s="58"/>
-      <c r="K17" s="58"/>
-      <c r="L17" s="58"/>
-      <c r="M17" s="58"/>
-      <c r="N17" s="58"/>
-      <c r="O17" s="58"/>
-      <c r="P17" s="58"/>
-      <c r="S17" s="58"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="M17" s="25"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="25"/>
+      <c r="S17" s="25"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1896,56 +1919,56 @@
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="6"/>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="46" t="s">
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="J10" s="43" t="s">
+      <c r="J10" s="53" t="s">
         <v>44</v>
       </c>
       <c r="K10" s="8"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="6"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="44"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="54"/>
       <c r="K11" s="8"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="6"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="44"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="54"/>
       <c r="K12" s="8"/>
     </row>
     <row r="13" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="6"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="45"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="55"/>
       <c r="K13" s="8"/>
     </row>
     <row r="14" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1980,14 +2003,14 @@
     </row>
     <row r="16" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="52" t="s">
+      <c r="C16" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="53"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="53"/>
-      <c r="H16" s="54"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="40"/>
       <c r="I16" s="23" t="s">
         <v>41</v>
       </c>
@@ -1998,14 +2021,14 @@
     </row>
     <row r="17" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="6"/>
-      <c r="C17" s="52" t="s">
+      <c r="C17" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="54"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="40"/>
       <c r="I17" s="23" t="s">
         <v>39</v>
       </c>
@@ -2016,14 +2039,14 @@
     </row>
     <row r="18" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="6"/>
-      <c r="C18" s="52" t="s">
+      <c r="C18" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="53"/>
-      <c r="H18" s="54"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="40"/>
       <c r="I18" s="23" t="s">
         <v>40</v>
       </c>
@@ -2034,14 +2057,14 @@
     </row>
     <row r="19" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="6"/>
-      <c r="C19" s="52" t="s">
+      <c r="C19" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="53"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="53"/>
-      <c r="H19" s="54"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="40"/>
       <c r="I19" s="23" t="s">
         <v>36</v>
       </c>
@@ -2052,108 +2075,108 @@
     </row>
     <row r="20" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="6"/>
-      <c r="C20" s="55"/>
-      <c r="D20" s="56"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="57"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="60"/>
+      <c r="H20" s="61"/>
       <c r="I20" s="19"/>
       <c r="J20" s="20"/>
       <c r="K20" s="8"/>
     </row>
     <row r="21" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="6"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="51"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="43"/>
       <c r="I21" s="19"/>
       <c r="J21" s="20"/>
       <c r="K21" s="8"/>
     </row>
     <row r="22" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="6"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="50"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="51"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="43"/>
       <c r="I22" s="19"/>
       <c r="J22" s="20"/>
       <c r="K22" s="8"/>
     </row>
     <row r="23" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="6"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="51"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="43"/>
       <c r="I23" s="19"/>
       <c r="J23" s="20"/>
       <c r="K23" s="8"/>
     </row>
     <row r="24" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="6"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="50"/>
-      <c r="G24" s="50"/>
-      <c r="H24" s="51"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="43"/>
       <c r="I24" s="19"/>
       <c r="J24" s="20"/>
       <c r="K24" s="8"/>
     </row>
     <row r="25" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="6"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="51"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="43"/>
       <c r="I25" s="19"/>
       <c r="J25" s="20"/>
       <c r="K25" s="8"/>
     </row>
     <row r="26" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="6"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="50"/>
-      <c r="G26" s="50"/>
-      <c r="H26" s="51"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="43"/>
       <c r="I26" s="19"/>
       <c r="J26" s="20"/>
       <c r="K26" s="8"/>
     </row>
     <row r="27" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="6"/>
-      <c r="C27" s="49"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="50"/>
-      <c r="H27" s="51"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="43"/>
       <c r="I27" s="19"/>
       <c r="J27" s="20"/>
       <c r="K27" s="8"/>
     </row>
     <row r="28" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="6"/>
-      <c r="C28" s="52"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="53"/>
-      <c r="F28" s="53"/>
-      <c r="G28" s="53"/>
-      <c r="H28" s="54"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="40"/>
       <c r="I28" s="21"/>
       <c r="J28" s="22"/>
       <c r="K28" s="8"/>
@@ -2172,11 +2195,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="C24:H24"/>
-    <mergeCell ref="C25:H25"/>
     <mergeCell ref="C10:H13"/>
     <mergeCell ref="J10:J13"/>
     <mergeCell ref="I10:I13"/>
@@ -2188,6 +2206,11 @@
     <mergeCell ref="C19:H19"/>
     <mergeCell ref="C20:H20"/>
     <mergeCell ref="C21:H21"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="C25:H25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Presentation and materials updated
</commit_message>
<xml_diff>
--- a/Ideas.xlsx
+++ b/Ideas.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dawwe\Desktop\Masters 2019-2020\Internet Tech\ITechGroupProject\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE75A1B-FC03-44F9-8F41-C9D638FA1CB6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74E6598-F037-40F7-AE3B-621EE9DA7E4B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1488" yWindow="204" windowWidth="21300" windowHeight="11508" activeTab="2" xr2:uid="{A4C79C33-EE3B-4DD3-8488-EB71656D6969}"/>
+    <workbookView minimized="1" xWindow="1488" yWindow="204" windowWidth="21300" windowHeight="11508" activeTab="3" xr2:uid="{A4C79C33-EE3B-4DD3-8488-EB71656D6969}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="ER tables" sheetId="3" r:id="rId2"/>
     <sheet name="ER tables UPDATED" sheetId="5" r:id="rId3"/>
-    <sheet name="Rating" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId4"/>
+    <sheet name="Rating" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ER tables UPDATED'!$K$2:$M$8</definedName>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="143">
   <si>
     <t>Stuff to do</t>
   </si>
@@ -337,6 +338,135 @@
   </si>
   <si>
     <t>linkOther</t>
+  </si>
+  <si>
+    <t>path('', views.IndexView.as_view(), name='index'),</t>
+  </si>
+  <si>
+    <t>path('about/', views.AboutView.as_view(), name='about'),</t>
+  </si>
+  <si>
+    <t>path('contact/', views.ContactView.as_view(), name='contact'),</t>
+  </si>
+  <si>
+    <t>path('playlist/&lt;slug:playlist_name_slug&gt;/', views.ShowPlaylistView.as_view(), name='show_playlist'),</t>
+  </si>
+  <si>
+    <t>path('add_playlist/', views.AddPlaylistView.as_view(), name='add_playlist'),</t>
+  </si>
+  <si>
+    <t>path('list_playlists/', views.ListPlaylistView.as_view(), name='list_playlists'),</t>
+  </si>
+  <si>
+    <t>path('playlist/&lt;slug:playlist_name_slug&gt;/rate_playlist/', views.PlaylistRatingView.as_view(), name='rate_playlist'),</t>
+  </si>
+  <si>
+    <t>path('playlist/&lt;slug:playlist_name_slug&gt;/edit_playlist/', views.PlaylistEditorView.as_view(), name='edit_playlist'),</t>
+  </si>
+  <si>
+    <t>path('playlist/&lt;slug:playlist_name_slug&gt;/edit_playlist/add_song/', views.AddSongView.as_view(), name='add_song'),</t>
+  </si>
+  <si>
+    <t>path('playlist/&lt;slug:playlist_name_slug&gt;/edit_playlist/remove_song/', views.RemoveSongView.as_view(), name='remove_song'),</t>
+  </si>
+  <si>
+    <t>path('playlist/&lt;slug:playlist_name_slug&gt;/edit_playlist/delete_playlist/', views.DeletePlaylistView.as_view(), name='delete_playlist'),</t>
+  </si>
+  <si>
+    <t>path('playlist/&lt;slug:playlist_name_slug&gt;/import/', views.ImportPlaylistView.as_view(), name='import_playlist'),</t>
+  </si>
+  <si>
+    <t>path('search_spotify/', views.SearchSpotifyView.as_view(), name='search_spotify'),</t>
+  </si>
+  <si>
+    <t>path('register_profile/', views.RegisterProfileView.as_view(), name='register_profile'),</t>
+  </si>
+  <si>
+    <t>path('profile/&lt;username&gt;/', views.ProfileView.as_view(), name='profile'),</t>
+  </si>
+  <si>
+    <t>path('profile/&lt;username&gt;/my_stats', views.MyStatsView.as_view(), name='my_stats'),</t>
+  </si>
+  <si>
+    <t>path('all_profiles/', views.ListProfileView.as_view(), name='list_profiles'),</t>
+  </si>
+  <si>
+    <t>path('publish_playlist/', views.PublishPlaylistView.as_view(), name='publish_playlist'),</t>
+  </si>
+  <si>
+    <t>path('suggest_tag/', views.TagSuggestionView.as_view(), name='suggest_tag'),</t>
+  </si>
+  <si>
+    <t>path('suggest_playlist/', views.PlaylistSuggestionView.as_view(), name='suggest_playlist'),</t>
+  </si>
+  <si>
+    <t>path('filter_playlists/', views.PlaylistFilterView.as_view(), name='filter_playlists'),</t>
+  </si>
+  <si>
+    <t>path('add_new_song_details/', views.AddSongDetailView.as_view(), name='add_new_song_details'),</t>
+  </si>
+  <si>
+    <t>about/</t>
+  </si>
+  <si>
+    <t>contact/</t>
+  </si>
+  <si>
+    <t>playlist/&lt;slug:playlist_name_slug&gt;/</t>
+  </si>
+  <si>
+    <t>add_playlist/</t>
+  </si>
+  <si>
+    <t>list_playlists/</t>
+  </si>
+  <si>
+    <t>playlist/&lt;slug:playlist_name_slug&gt;/rate_playlist/</t>
+  </si>
+  <si>
+    <t>playlist/&lt;slug:playlist_name_slug&gt;/edit_playlist/</t>
+  </si>
+  <si>
+    <t>playlist/&lt;slug:playlist_name_slug&gt;/edit_playlist/add_song/</t>
+  </si>
+  <si>
+    <t>playlist/&lt;slug:playlist_name_slug&gt;/edit_playlist/remove_song/</t>
+  </si>
+  <si>
+    <t>playlist/&lt;slug:playlist_name_slug&gt;/edit_playlist/delete_playlist/</t>
+  </si>
+  <si>
+    <t>playlist/&lt;slug:playlist_name_slug&gt;/import/</t>
+  </si>
+  <si>
+    <t>search_spotify/</t>
+  </si>
+  <si>
+    <t>register_profile/</t>
+  </si>
+  <si>
+    <t>profile/&lt;username&gt;/</t>
+  </si>
+  <si>
+    <t>profile/&lt;username&gt;/my_stats</t>
+  </si>
+  <si>
+    <t>all_profiles/</t>
+  </si>
+  <si>
+    <t>publish_playlist/</t>
+  </si>
+  <si>
+    <t>suggest_tag/</t>
+  </si>
+  <si>
+    <t>suggest_playlist/</t>
+  </si>
+  <si>
+    <t>filter_playlists/</t>
+  </si>
+  <si>
+    <t>add_new_song_details/</t>
   </si>
 </sst>
 </file>
@@ -680,6 +810,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -707,6 +839,60 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -716,60 +902,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -779,8 +911,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1161,82 +1291,82 @@
       <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="32"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="34"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="33"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="37"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="33"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="37"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D14" s="33"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="37"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D15" s="33"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="37"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D16" s="33"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="37"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="33"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="37"/>
     </row>
     <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="36"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="40"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
@@ -1913,8 +2043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFD37BFE-509C-43C6-9A98-8EE5A2937C67}">
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="S26" sqref="S26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2061,10 +2191,10 @@
         <v>60</v>
       </c>
       <c r="J4" s="25"/>
-      <c r="K4" s="63" t="s">
+      <c r="K4" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="L4" s="63" t="s">
+      <c r="L4" s="30" t="s">
         <v>94</v>
       </c>
       <c r="M4" s="25"/>
@@ -2106,10 +2236,10 @@
         <v>80</v>
       </c>
       <c r="J5" s="25"/>
-      <c r="K5" s="64" t="s">
+      <c r="K5" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="L5" s="64" t="s">
+      <c r="L5" s="31" t="s">
         <v>60</v>
       </c>
       <c r="M5" s="25"/>
@@ -2120,10 +2250,10 @@
         <v>70</v>
       </c>
       <c r="P5" s="25"/>
-      <c r="Q5" s="63" t="s">
+      <c r="Q5" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="R5" s="63" t="s">
+      <c r="R5" s="30" t="s">
         <v>94</v>
       </c>
       <c r="S5" s="25"/>
@@ -2147,14 +2277,14 @@
       <c r="H6" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="I6" s="63" t="s">
+      <c r="I6" s="30" t="s">
         <v>62</v>
       </c>
       <c r="J6" s="25"/>
-      <c r="K6" s="64" t="s">
+      <c r="K6" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="L6" s="64" t="s">
+      <c r="L6" s="31" t="s">
         <v>70</v>
       </c>
       <c r="M6" s="25"/>
@@ -2184,14 +2314,14 @@
       <c r="H7" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="I7" s="63" t="s">
+      <c r="I7" s="30" t="s">
         <v>97</v>
       </c>
       <c r="J7" s="25"/>
-      <c r="K7" s="64" t="s">
+      <c r="K7" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="L7" s="64" t="s">
+      <c r="L7" s="31" t="s">
         <v>70</v>
       </c>
       <c r="M7" s="25"/>
@@ -2221,17 +2351,17 @@
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
       <c r="J8" s="25"/>
-      <c r="K8" s="64" t="s">
+      <c r="K8" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="L8" s="64" t="s">
+      <c r="L8" s="31" t="s">
         <v>73</v>
       </c>
       <c r="M8" s="25"/>
-      <c r="N8" s="63" t="s">
+      <c r="N8" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="O8" s="63" t="s">
+      <c r="O8" s="30" t="s">
         <v>94</v>
       </c>
       <c r="P8" s="25"/>
@@ -2269,7 +2399,7 @@
       <c r="B10" s="25"/>
       <c r="C10" s="25"/>
       <c r="D10" s="25"/>
-      <c r="E10" s="63" t="s">
+      <c r="E10" s="30" t="s">
         <v>96</v>
       </c>
       <c r="F10" s="27" t="s">
@@ -2297,7 +2427,7 @@
       <c r="E11" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="63" t="s">
+      <c r="F11" s="30" t="s">
         <v>95</v>
       </c>
       <c r="G11" s="25"/>
@@ -2322,7 +2452,7 @@
       <c r="E12" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="63" t="s">
+      <c r="F12" s="30" t="s">
         <v>95</v>
       </c>
       <c r="G12" s="25"/>
@@ -2347,7 +2477,7 @@
       <c r="E13" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="F13" s="63" t="s">
+      <c r="F13" s="30" t="s">
         <v>97</v>
       </c>
       <c r="G13" s="25"/>
@@ -2372,7 +2502,7 @@
       <c r="E14" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="F14" s="63" t="s">
+      <c r="F14" s="30" t="s">
         <v>97</v>
       </c>
       <c r="G14" s="25"/>
@@ -2394,10 +2524,10 @@
       <c r="B15" s="25"/>
       <c r="C15" s="25"/>
       <c r="D15" s="25"/>
-      <c r="E15" s="63" t="s">
+      <c r="E15" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="F15" s="63" t="s">
+      <c r="F15" s="30" t="s">
         <v>94</v>
       </c>
       <c r="G15" s="25"/>
@@ -2419,10 +2549,10 @@
       <c r="B16" s="25"/>
       <c r="C16" s="25"/>
       <c r="D16" s="25"/>
-      <c r="E16" s="64" t="s">
+      <c r="E16" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="F16" s="64" t="s">
+      <c r="F16" s="31" t="s">
         <v>57</v>
       </c>
       <c r="G16" s="25"/>
@@ -2566,17 +2696,208 @@
       <c r="S22" s="25"/>
     </row>
   </sheetData>
-  <autoFilter ref="K2:M8" xr:uid="{70F3C947-6DC4-4E32-B9CF-4BAE555AE5E4}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K3:M8">
-      <sortCondition ref="M2:M8"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F05010-A275-4B00-8BBA-6BE3380A46A1}">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="109.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" t="str">
+        <f>MID(A1,8,10)</f>
+        <v>, views.In</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>113</v>
+      </c>
+      <c r="B14" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>114</v>
+      </c>
+      <c r="B15" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>118</v>
+      </c>
+      <c r="B19" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>119</v>
+      </c>
+      <c r="B20" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>121</v>
+      </c>
+      <c r="B22" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E112665-A4DD-420C-8380-223FF5B10D2A}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:K29"/>
@@ -2704,56 +3025,56 @@
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="6"/>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="57" t="s">
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="J10" s="54" t="s">
+      <c r="J10" s="50" t="s">
         <v>44</v>
       </c>
       <c r="K10" s="8"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="6"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="55"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="51"/>
       <c r="K11" s="8"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="6"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="55"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="51"/>
       <c r="K12" s="8"/>
     </row>
     <row r="13" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="6"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="56"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="52"/>
       <c r="K13" s="8"/>
     </row>
     <row r="14" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2788,14 +3109,14 @@
     </row>
     <row r="16" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="41"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="61"/>
       <c r="I16" s="23" t="s">
         <v>41</v>
       </c>
@@ -2806,14 +3127,14 @@
     </row>
     <row r="17" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="6"/>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="41"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="61"/>
       <c r="I17" s="23" t="s">
         <v>39</v>
       </c>
@@ -2824,14 +3145,14 @@
     </row>
     <row r="18" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="6"/>
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="41"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="61"/>
       <c r="I18" s="23" t="s">
         <v>40</v>
       </c>
@@ -2842,14 +3163,14 @@
     </row>
     <row r="19" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="6"/>
-      <c r="C19" s="39" t="s">
+      <c r="C19" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="41"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="61"/>
       <c r="I19" s="23" t="s">
         <v>36</v>
       </c>
@@ -2860,108 +3181,108 @@
     </row>
     <row r="20" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="6"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="61"/>
-      <c r="E20" s="61"/>
-      <c r="F20" s="61"/>
-      <c r="G20" s="61"/>
-      <c r="H20" s="62"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="64"/>
       <c r="I20" s="19"/>
       <c r="J20" s="20"/>
       <c r="K20" s="8"/>
     </row>
     <row r="21" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="6"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="44"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="57"/>
+      <c r="H21" s="58"/>
       <c r="I21" s="19"/>
       <c r="J21" s="20"/>
       <c r="K21" s="8"/>
     </row>
     <row r="22" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="6"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="44"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="58"/>
       <c r="I22" s="19"/>
       <c r="J22" s="20"/>
       <c r="K22" s="8"/>
     </row>
     <row r="23" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="6"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="44"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="58"/>
       <c r="I23" s="19"/>
       <c r="J23" s="20"/>
       <c r="K23" s="8"/>
     </row>
     <row r="24" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="6"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="44"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="58"/>
       <c r="I24" s="19"/>
       <c r="J24" s="20"/>
       <c r="K24" s="8"/>
     </row>
     <row r="25" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="6"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="44"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="58"/>
       <c r="I25" s="19"/>
       <c r="J25" s="20"/>
       <c r="K25" s="8"/>
     </row>
     <row r="26" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="6"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="44"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="58"/>
       <c r="I26" s="19"/>
       <c r="J26" s="20"/>
       <c r="K26" s="8"/>
     </row>
     <row r="27" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="6"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="44"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="57"/>
+      <c r="H27" s="58"/>
       <c r="I27" s="19"/>
       <c r="J27" s="20"/>
       <c r="K27" s="8"/>
     </row>
     <row r="28" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="6"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="40"/>
-      <c r="F28" s="40"/>
-      <c r="G28" s="40"/>
-      <c r="H28" s="41"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="60"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="60"/>
+      <c r="H28" s="61"/>
       <c r="I28" s="21"/>
       <c r="J28" s="22"/>
       <c r="K28" s="8"/>
@@ -2980,6 +3301,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="C25:H25"/>
     <mergeCell ref="C10:H13"/>
     <mergeCell ref="J10:J13"/>
     <mergeCell ref="I10:I13"/>
@@ -2991,11 +3317,6 @@
     <mergeCell ref="C19:H19"/>
     <mergeCell ref="C20:H20"/>
     <mergeCell ref="C21:H21"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="C24:H24"/>
-    <mergeCell ref="C25:H25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>